<commit_message>
update UVM verification platform-doc-vplan files
</commit_message>
<xml_diff>
--- a/kei_i2c_tb/doc/questa_vplan.xlsx
+++ b/kei_i2c_tb/doc/questa_vplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDA\project\I2C\I2C\kei_i2c_tb\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4577604A-BD52-4EB2-A278-95B7A9ADF8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0A25B-3634-4D0F-802E-A13AA68397C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="1" xr2:uid="{5E2C75AA-68D8-4CB5-A34E-2C4947224CD1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
   <si>
     <t>Section</t>
   </si>
@@ -378,6 +378,39 @@
   </si>
   <si>
     <t>kei_i2c_reg_access_test_*</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>test status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All tests status and pass rate recorded</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">kei_i2c_reg_access_test_*
+kei_i2c_reg_bit_bash_test_*
+kei_i2c_reg_hw_reset_test_*       
+kei_i2c_quick_reg_access_test_*
+kei_i2c_master_directed_write_packet_test_*
+kei_i2c_master_directed_read_packet_test_*
+kei_i2c_master_directed_interrupt_test_*
+kei_i2c_master_address_cg_test_*
+kei_i2c_master_ss_cnt_test_*
+kei_i2c_master_fs_cnt_test_*
+kei_i2c_master_hs_cnt_test_*
+kei_i2c_master_sda_control_cg_test_*
+kei_i2c_master_timeout_cg_test_*
+kei_i2c_master_enabled_cg_test_*
+kei_i2c_master_stop_det_intr_test_*
+kei_i2c_master_tx_abrt_intr_test_*
+kei_i2c_master_rx_full_intr_test_*
+kei_i2c_master_rx_over_intr_test_*
+</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -862,23 +895,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F0FA01-3D0B-4284-9FC5-DD3914B6A82B}">
-  <dimension ref="B3:H25"/>
+  <dimension ref="B3:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.35546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="50.640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.35546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.92578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.0703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
@@ -1383,6 +1416,29 @@
         <v>1</v>
       </c>
       <c r="H25" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="268.75" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="15">
+        <v>1</v>
+      </c>
+      <c r="H26" s="14">
         <v>100</v>
       </c>
     </row>

</xml_diff>